<commit_message>
made proxy for individual heat PJ
</commit_message>
<xml_diff>
--- a/data/energy2050-2035.xlsx
+++ b/data/energy2050-2035.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="individual heat" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="district heat" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="capacity per energy" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="61">
   <si>
     <t xml:space="preserve">https://ens.dk/sites/ens.dk/files/Basisfremskrivning/energiscenarier_-_analyse_2014_web.pdf, table 10.7 and 10.8</t>
   </si>
@@ -128,9 +129,6 @@
     <t xml:space="preserve">KeroseneHydrogeneration</t>
   </si>
   <si>
-    <t xml:space="preserve">District heat use</t>
-  </si>
-  <si>
     <t xml:space="preserve">decentral DH</t>
   </si>
   <si>
@@ -183,6 +181,30 @@
   </si>
   <si>
     <t xml:space="preserve">Wood chips CHP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DH capacity (MW)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ens.dk/service/fremskrivninger-analyser-modeller/scenarieanalysen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DH energy (PJ)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ens.dk/service/fremskrivninger-analyser-modeller/analyseforudsaetninger-til-energinet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IH capacity (MW)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IH energy (PJ)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">assuming ratio between energy and capacity the same for DH and IH</t>
   </si>
 </sst>
 </file>
@@ -197,7 +219,7 @@
     <numFmt numFmtId="168" formatCode="0.00%"/>
     <numFmt numFmtId="169" formatCode="0"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -222,6 +244,26 @@
     <font>
       <b val="true"/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF080808"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -275,7 +317,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -317,6 +359,18 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -409,7 +463,7 @@
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF080808"/>
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
@@ -431,7 +485,7 @@
       <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -732,11 +786,11 @@
   </sheetPr>
   <dimension ref="A1:AA74"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I27" activeCellId="0" sqref="I27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="W14" activeCellId="0" sqref="W14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -796,23 +850,23 @@
         <f aca="false">F7</f>
         <v>Hydrogen</v>
       </c>
-      <c r="W2" s="0" t="str">
+      <c r="W2" s="5" t="str">
         <f aca="false">L2</f>
         <v>2050 combined district heat</v>
       </c>
-      <c r="X2" s="0" t="str">
+      <c r="X2" s="5" t="str">
         <f aca="false">M2</f>
         <v>Wind</v>
       </c>
-      <c r="Y2" s="0" t="str">
+      <c r="Y2" s="5" t="str">
         <f aca="false">N2</f>
         <v>Biomass</v>
       </c>
-      <c r="Z2" s="0" t="str">
+      <c r="Z2" s="5" t="str">
         <f aca="false">O2</f>
         <v>Bio+</v>
       </c>
-      <c r="AA2" s="0" t="str">
+      <c r="AA2" s="5" t="str">
         <f aca="false">P2</f>
         <v>Hydrogen</v>
       </c>
@@ -855,13 +909,13 @@
       </c>
       <c r="T3" s="8" t="n">
         <f aca="false">O3/SUM(O$3:O$24)</f>
-        <v>0.14413392251235</v>
+        <v>0.144096076314865</v>
       </c>
       <c r="U3" s="8" t="n">
         <f aca="false">P3/SUM(P$3:P$24)</f>
         <v>0</v>
       </c>
-      <c r="W3" s="0" t="str">
+      <c r="W3" s="5" t="str">
         <f aca="false">L3</f>
         <v>Woodchips CHP</v>
       </c>
@@ -926,23 +980,23 @@
         <f aca="false">P4/SUM(P$3:P$24)</f>
         <v>0</v>
       </c>
-      <c r="W4" s="0" t="str">
+      <c r="W4" s="5" t="str">
         <f aca="false">L4</f>
         <v>Gas CHP</v>
       </c>
-      <c r="X4" s="0" t="n">
+      <c r="X4" s="5" t="n">
         <f aca="false">M4+M5+M6</f>
         <v>4.87728</v>
       </c>
-      <c r="Y4" s="0" t="n">
+      <c r="Y4" s="5" t="n">
         <f aca="false">N4+N5+N6</f>
         <v>6.19704</v>
       </c>
-      <c r="Z4" s="0" t="n">
+      <c r="Z4" s="5" t="n">
         <f aca="false">O4+O5+O6</f>
         <v>6.07392</v>
       </c>
-      <c r="AA4" s="0" t="n">
+      <c r="AA4" s="5" t="n">
         <f aca="false">P4+P5+P6</f>
         <v>3.94848</v>
       </c>
@@ -977,21 +1031,21 @@
       </c>
       <c r="R5" s="8" t="n">
         <f aca="false">M5/SUM(M$3:M$24)</f>
-        <v>0.0645070793519924</v>
+        <v>0.0644884964574643</v>
       </c>
       <c r="S5" s="8" t="n">
         <f aca="false">N5/SUM(N$3:N$24)</f>
-        <v>0.0729270103319196</v>
+        <v>0.0729083171770157</v>
       </c>
       <c r="T5" s="8" t="n">
         <f aca="false">O5/SUM(O$3:O$24)</f>
-        <v>0.0732213519399123</v>
+        <v>0.0732021257251716</v>
       </c>
       <c r="U5" s="8" t="n">
         <f aca="false">P5/SUM(P$3:P$24)</f>
-        <v>0.0500568136620051</v>
-      </c>
-      <c r="W5" s="0" t="str">
+        <v>0.0500429914375292</v>
+      </c>
+      <c r="W5" s="5" t="str">
         <f aca="false">L7</f>
         <v>Waste CHP</v>
       </c>
@@ -1065,7 +1119,7 @@
         <f aca="false">P6/SUM(P$3:P$24)</f>
         <v>0</v>
       </c>
-      <c r="W6" s="0" t="str">
+      <c r="W6" s="5" t="str">
         <f aca="false">L8</f>
         <v>Biomass</v>
       </c>
@@ -1135,37 +1189,37 @@
       </c>
       <c r="R7" s="8" t="n">
         <f aca="false">M7/SUM(M$3:M$24)</f>
-        <v>0.389908822566774</v>
+        <v>0.389796499476067</v>
       </c>
       <c r="S7" s="8" t="n">
         <f aca="false">N7/SUM(N$3:N$24)</f>
-        <v>0.357644836308856</v>
+        <v>0.357553162314608</v>
       </c>
       <c r="T7" s="8" t="n">
         <f aca="false">O7/SUM(O$3:O$24)</f>
-        <v>0.365412389363479</v>
+        <v>0.365316440615188</v>
       </c>
       <c r="U7" s="8" t="n">
         <f aca="false">P7/SUM(P$3:P$24)</f>
-        <v>0.370360177668828</v>
-      </c>
-      <c r="W7" s="0" t="str">
+        <v>0.370257909842769</v>
+      </c>
+      <c r="W7" s="5" t="str">
         <f aca="false">L10</f>
         <v>heat pumps</v>
       </c>
-      <c r="X7" s="0" t="n">
+      <c r="X7" s="5" t="n">
         <f aca="false">M10</f>
         <v>17.82054</v>
       </c>
-      <c r="Y7" s="0" t="n">
+      <c r="Y7" s="5" t="n">
         <f aca="false">N10</f>
         <v>19.94994</v>
       </c>
-      <c r="Z7" s="0" t="n">
+      <c r="Z7" s="5" t="n">
         <f aca="false">O10</f>
         <v>4.90032</v>
       </c>
-      <c r="AA7" s="0" t="n">
+      <c r="AA7" s="5" t="n">
         <f aca="false">P10</f>
         <v>27.0648</v>
       </c>
@@ -1223,33 +1277,33 @@
       </c>
       <c r="S8" s="8" t="n">
         <f aca="false">N8/SUM(N$3:N$24)</f>
-        <v>0.0495500356013786</v>
+        <v>0.0495373345940732</v>
       </c>
       <c r="T8" s="8" t="n">
         <f aca="false">O8/SUM(O$3:O$24)</f>
-        <v>0.045307664429391</v>
+        <v>0.0452957676962299</v>
       </c>
       <c r="U8" s="8" t="n">
         <f aca="false">P8/SUM(P$3:P$24)</f>
         <v>0</v>
       </c>
-      <c r="W8" s="0" t="str">
+      <c r="W8" s="5" t="str">
         <f aca="false">L11</f>
         <v>Geothermal</v>
       </c>
-      <c r="X8" s="0" t="n">
+      <c r="X8" s="5" t="n">
         <f aca="false">M11</f>
         <v>4.19004</v>
       </c>
-      <c r="Y8" s="0" t="n">
+      <c r="Y8" s="5" t="n">
         <f aca="false">N11</f>
         <v>4.46508</v>
       </c>
-      <c r="Z8" s="0" t="n">
+      <c r="Z8" s="5" t="n">
         <f aca="false">O11</f>
         <v>3.15216</v>
       </c>
-      <c r="AA8" s="0" t="n">
+      <c r="AA8" s="5" t="n">
         <f aca="false">P11</f>
         <v>4.43844</v>
       </c>
@@ -1317,23 +1371,23 @@
         <f aca="false">P9/SUM(P$3:P$24)</f>
         <v>0</v>
       </c>
-      <c r="W9" s="0" t="str">
+      <c r="W9" s="5" t="str">
         <f aca="false">L12</f>
         <v>Solar heat</v>
       </c>
-      <c r="X9" s="0" t="n">
+      <c r="X9" s="5" t="n">
         <f aca="false">M12</f>
         <v>7</v>
       </c>
-      <c r="Y9" s="0" t="n">
+      <c r="Y9" s="5" t="n">
         <f aca="false">N12</f>
         <v>7</v>
       </c>
-      <c r="Z9" s="0" t="n">
+      <c r="Z9" s="5" t="n">
         <f aca="false">O12</f>
         <v>7</v>
       </c>
-      <c r="AA9" s="0" t="n">
+      <c r="AA9" s="5" t="n">
         <f aca="false">P12</f>
         <v>7</v>
       </c>
@@ -1388,37 +1442,37 @@
       </c>
       <c r="R10" s="8" t="n">
         <f aca="false">M10/SUM(M$3:M$24)</f>
-        <v>0.235695098061902</v>
+        <v>0.235627200132061</v>
       </c>
       <c r="S10" s="8" t="n">
         <f aca="false">N10/SUM(N$3:N$24)</f>
-        <v>0.234771678172349</v>
+        <v>0.234711499874526</v>
       </c>
       <c r="T10" s="8" t="n">
         <f aca="false">O10/SUM(O$3:O$24)</f>
-        <v>0.0590735563422289</v>
+        <v>0.0590580450077664</v>
       </c>
       <c r="U10" s="8" t="n">
         <f aca="false">P10/SUM(P$3:P$24)</f>
-        <v>0.343113717278404</v>
-      </c>
-      <c r="W10" s="0" t="str">
+        <v>0.343018973037331</v>
+      </c>
+      <c r="W10" s="5" t="str">
         <f aca="false">L13</f>
         <v>Residual industrial heat</v>
       </c>
-      <c r="X10" s="0" t="n">
+      <c r="X10" s="5" t="n">
         <f aca="false">M13</f>
         <v>4.7</v>
       </c>
-      <c r="Y10" s="0" t="n">
+      <c r="Y10" s="5" t="n">
         <f aca="false">N13</f>
         <v>4.7</v>
       </c>
-      <c r="Z10" s="0" t="n">
+      <c r="Z10" s="5" t="n">
         <f aca="false">O13</f>
         <v>4.7</v>
       </c>
-      <c r="AA10" s="0" t="n">
+      <c r="AA10" s="5" t="n">
         <f aca="false">P13</f>
         <v>4.7</v>
       </c>
@@ -1473,37 +1527,37 @@
       </c>
       <c r="R11" s="8" t="n">
         <f aca="false">M11/SUM(M$3:M$24)</f>
-        <v>0.0554176185841334</v>
+        <v>0.0554016541385021</v>
       </c>
       <c r="S11" s="8" t="n">
         <f aca="false">N11/SUM(N$3:N$24)</f>
-        <v>0.0525452369668176</v>
+        <v>0.0525317682088141</v>
       </c>
       <c r="T11" s="8" t="n">
         <f aca="false">O11/SUM(O$3:O$24)</f>
-        <v>0.0379994166421214</v>
+        <v>0.0379894388839262</v>
       </c>
       <c r="U11" s="8" t="n">
         <f aca="false">P11/SUM(P$3:P$24)</f>
-        <v>0.0562682764076277</v>
-      </c>
-      <c r="W11" s="0" t="str">
+        <v>0.0562527390074122</v>
+      </c>
+      <c r="W11" s="5" t="str">
         <f aca="false">L14</f>
         <v>Wood boiler</v>
       </c>
-      <c r="X11" s="0" t="n">
+      <c r="X11" s="5" t="n">
         <f aca="false">M14</f>
         <v>0</v>
       </c>
-      <c r="Y11" s="0" t="n">
+      <c r="Y11" s="5" t="n">
         <f aca="false">N14</f>
         <v>8.08056</v>
       </c>
-      <c r="Z11" s="0" t="n">
+      <c r="Z11" s="5" t="n">
         <f aca="false">O14</f>
         <v>11.10528</v>
       </c>
-      <c r="AA11" s="0" t="n">
+      <c r="AA11" s="5" t="n">
         <f aca="false">P14</f>
         <v>0</v>
       </c>
@@ -1558,37 +1612,37 @@
       </c>
       <c r="R12" s="8" t="n">
         <f aca="false">M12/SUM(M$3:M$24)</f>
-        <v>0.0925822498326827</v>
+        <v>0.0925555791757393</v>
       </c>
       <c r="S12" s="8" t="n">
         <f aca="false">N12/SUM(N$3:N$24)</f>
-        <v>0.0823762751770905</v>
+        <v>0.0823551599213673</v>
       </c>
       <c r="T12" s="8" t="n">
         <f aca="false">O12/SUM(O$3:O$24)</f>
-        <v>0.0843852838989296</v>
+        <v>0.0843631262967245</v>
       </c>
       <c r="U12" s="8" t="n">
         <f aca="false">P12/SUM(P$3:P$24)</f>
-        <v>0.088742426360026</v>
-      </c>
-      <c r="W12" s="0" t="str">
+        <v>0.0887179218490924</v>
+      </c>
+      <c r="W12" s="5" t="str">
         <f aca="false">L15</f>
         <v>Straw boiler</v>
       </c>
-      <c r="X12" s="0" t="n">
+      <c r="X12" s="5" t="n">
         <f aca="false">M15</f>
         <v>7.5582</v>
       </c>
-      <c r="Y12" s="0" t="n">
+      <c r="Y12" s="5" t="n">
         <f aca="false">N15</f>
         <v>0</v>
       </c>
-      <c r="Z12" s="0" t="n">
+      <c r="Z12" s="5" t="n">
         <f aca="false">O15</f>
         <v>0.0126</v>
       </c>
-      <c r="AA12" s="0" t="n">
+      <c r="AA12" s="5" t="n">
         <f aca="false">P15</f>
         <v>2.53296</v>
       </c>
@@ -1643,36 +1697,36 @@
       </c>
       <c r="R13" s="8" t="n">
         <f aca="false">M13/SUM(M$3:M$24)</f>
-        <v>0.0621623677448013</v>
+        <v>0.0621444603037107</v>
       </c>
       <c r="S13" s="8" t="n">
         <f aca="false">N13/SUM(N$3:N$24)</f>
-        <v>0.0553097847617608</v>
+        <v>0.0552956073757752</v>
       </c>
       <c r="T13" s="8" t="n">
         <f aca="false">O13/SUM(O$3:O$24)</f>
-        <v>0.0566586906178527</v>
+        <v>0.0566438133706579</v>
       </c>
       <c r="U13" s="8" t="n">
         <f aca="false">P13/SUM(P$3:P$24)</f>
-        <v>0.0595842005560175</v>
-      </c>
-      <c r="W13" s="0" t="s">
+        <v>0.0595677475272478</v>
+      </c>
+      <c r="W13" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="X13" s="0" t="n">
+      <c r="X13" s="5" t="n">
         <f aca="false">M17+M18+M19+M20+M21</f>
         <v>0.0032472</v>
       </c>
-      <c r="Y13" s="0" t="n">
+      <c r="Y13" s="5" t="n">
         <f aca="false">N17+N18+N19+N20+N21</f>
         <v>0.0039132</v>
       </c>
-      <c r="Z13" s="0" t="n">
+      <c r="Z13" s="5" t="n">
         <f aca="false">O17+O18+O19+O20+O21</f>
         <v>0.0042228</v>
       </c>
-      <c r="AA13" s="0" t="n">
+      <c r="AA13" s="5" t="n">
         <f aca="false">P17+P18+P19+P20+P21</f>
         <v>0.0025524</v>
       </c>
@@ -1731,35 +1785,15 @@
       </c>
       <c r="S14" s="8" t="n">
         <f aca="false">N14/SUM(N$3:N$24)</f>
-        <v>0.0950923477349986</v>
+        <v>0.0950679730077434</v>
       </c>
       <c r="T14" s="8" t="n">
         <f aca="false">O14/SUM(O$3:O$24)</f>
-        <v>0.133874600796729</v>
+        <v>0.133839448457213</v>
       </c>
       <c r="U14" s="8" t="n">
         <f aca="false">P14/SUM(P$3:P$24)</f>
         <v>0</v>
-      </c>
-      <c r="W14" s="0" t="str">
-        <f aca="false">L24</f>
-        <v>District heat use</v>
-      </c>
-      <c r="X14" s="0" t="n">
-        <f aca="false">M24</f>
-        <v>-0.0217872</v>
-      </c>
-      <c r="Y14" s="0" t="n">
-        <f aca="false">N24</f>
-        <v>-0.0217872</v>
-      </c>
-      <c r="Z14" s="0" t="n">
-        <f aca="false">O24</f>
-        <v>-0.0217872</v>
-      </c>
-      <c r="AA14" s="0" t="n">
-        <f aca="false">P24</f>
-        <v>-0.0217872</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1812,7 +1846,7 @@
       </c>
       <c r="R15" s="8" t="n">
         <f aca="false">M15/SUM(M$3:M$24)</f>
-        <v>0.0999650229550547</v>
+        <v>0.0999362255037248</v>
       </c>
       <c r="S15" s="8" t="n">
         <f aca="false">N15/SUM(N$3:N$24)</f>
@@ -1820,11 +1854,11 @@
       </c>
       <c r="T15" s="8" t="n">
         <f aca="false">O15/SUM(O$3:O$24)</f>
-        <v>0.000151893511018073</v>
+        <v>0.000151853627334104</v>
       </c>
       <c r="U15" s="8" t="n">
         <f aca="false">P15/SUM(P$3:P$24)</f>
-        <v>0.0321115737532702</v>
+        <v>0.0321027067609824</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1945,11 +1979,11 @@
       </c>
       <c r="S17" s="8" t="n">
         <f aca="false">N17/SUM(N$3:N$24)</f>
-        <v>1.02946807892741E-005</v>
+        <v>1.02920419856017E-005</v>
       </c>
       <c r="T17" s="8" t="n">
         <f aca="false">O17/SUM(O$3:O$24)</f>
-        <v>1.50591566637918E-005</v>
+        <v>1.50552024814098E-005</v>
       </c>
       <c r="U17" s="8" t="n">
         <f aca="false">P17/SUM(P$3:P$24)</f>
@@ -2011,11 +2045,11 @@
       </c>
       <c r="S18" s="8" t="n">
         <f aca="false">N18/SUM(N$3:N$24)</f>
-        <v>8.09170383025249E-006</v>
+        <v>8.08962970884745E-006</v>
       </c>
       <c r="T18" s="8" t="n">
         <f aca="false">O18/SUM(O$3:O$24)</f>
-        <v>7.50787925889333E-006</v>
+        <v>7.50590786537143E-006</v>
       </c>
       <c r="U18" s="8" t="n">
         <f aca="false">P18/SUM(P$3:P$24)</f>
@@ -2073,7 +2107,7 @@
       </c>
       <c r="R19" s="8" t="n">
         <f aca="false">M19/SUM(M$3:M$24)</f>
-        <v>1.73313971686782E-005</v>
+        <v>1.73264044216984E-005</v>
       </c>
       <c r="S19" s="8" t="n">
         <f aca="false">N19/SUM(N$3:N$24)</f>
@@ -2085,7 +2119,7 @@
       </c>
       <c r="U19" s="8" t="n">
         <f aca="false">P19/SUM(P$3:P$24)</f>
-        <v>7.80426252389029E-006</v>
+        <v>7.8021075271859E-006</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2143,11 +2177,11 @@
       </c>
       <c r="S20" s="8" t="n">
         <f aca="false">N20/SUM(N$3:N$24)</f>
-        <v>2.76643068123292E-005</v>
+        <v>2.76572157061643E-005</v>
       </c>
       <c r="T20" s="8" t="n">
         <f aca="false">O20/SUM(O$3:O$24)</f>
-        <v>2.83389893413719E-005</v>
+        <v>2.83315481854771E-005</v>
       </c>
       <c r="U20" s="8" t="n">
         <f aca="false">P20/SUM(P$3:P$24)</f>
@@ -2202,7 +2236,7 @@
       </c>
       <c r="R21" s="8" t="n">
         <f aca="false">M21/SUM(M$3:M$24)</f>
-        <v>2.56161859251343E-005</v>
+        <v>2.56088065353674E-005</v>
       </c>
       <c r="S21" s="8" t="n">
         <f aca="false">N21/SUM(N$3:N$24)</f>
@@ -2214,7 +2248,7 @@
       </c>
       <c r="U21" s="8" t="n">
         <f aca="false">P21/SUM(P$3:P$24)</f>
-        <v>2.45537616248712E-005</v>
+        <v>2.45469815767603E-005</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2268,41 +2302,29 @@
       </c>
       <c r="R22" s="8" t="n">
         <f aca="false">M22/SUM(M$3:M$24)</f>
-        <v>-7.71342401463151E-006</v>
+        <v>-7.71120196789874E-006</v>
       </c>
       <c r="S22" s="8" t="n">
         <f aca="false">N22/SUM(N$3:N$24)</f>
-        <v>-6.86312052618274E-006</v>
+        <v>-6.86136132373449E-006</v>
       </c>
       <c r="T22" s="8" t="n">
         <f aca="false">O22/SUM(O$3:O$24)</f>
-        <v>-7.03049965283653E-006</v>
+        <v>-7.02865360803568E-006</v>
       </c>
       <c r="U22" s="8" t="n">
         <f aca="false">P22/SUM(P$3:P$24)</f>
-        <v>-7.39351186473817E-006</v>
+        <v>-7.39147028891296E-006</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="7"/>
-      <c r="B23" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C23" s="7" t="n">
-        <v>-0.0130716</v>
-      </c>
-      <c r="D23" s="7" t="n">
-        <v>-0.0130716</v>
-      </c>
-      <c r="E23" s="7" t="n">
-        <v>-0.0130716</v>
-      </c>
-      <c r="F23" s="7" t="n">
-        <v>-0.0130716</v>
-      </c>
-      <c r="G23" s="7" t="n">
-        <v>-0.0130716</v>
-      </c>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
       <c r="J23" s="5" t="s">
         <v>17</v>
       </c>
@@ -2332,7 +2354,7 @@
       </c>
       <c r="R23" s="8" t="n">
         <f aca="false">M23/SUM(M$3:M$24)</f>
-        <v>1.46650283734969E-005</v>
+        <v>1.46608037414371E-005</v>
       </c>
       <c r="S23" s="8" t="n">
         <f aca="false">N23/SUM(N$3:N$24)</f>
@@ -2344,7 +2366,7 @@
       </c>
       <c r="U23" s="8" t="n">
         <f aca="false">P23/SUM(P$3:P$24)</f>
-        <v>1.40568003354281E-005</v>
+        <v>1.40529188208962E-005</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2355,49 +2377,28 @@
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
-      <c r="J24" s="5" t="str">
-        <f aca="false">B23</f>
-        <v>District heat use</v>
-      </c>
-      <c r="K24" s="5" t="str">
-        <f aca="false">B40</f>
-        <v>District heat use</v>
-      </c>
-      <c r="L24" s="6" t="str">
-        <f aca="false">K24</f>
-        <v>District heat use</v>
-      </c>
-      <c r="M24" s="5" t="n">
-        <f aca="false">C23+C40</f>
-        <v>-0.0217872</v>
-      </c>
-      <c r="N24" s="5" t="n">
-        <f aca="false">D23+D40</f>
-        <v>-0.0217872</v>
-      </c>
-      <c r="O24" s="5" t="n">
-        <f aca="false">E23+E40</f>
-        <v>-0.0217872</v>
-      </c>
-      <c r="P24" s="5" t="n">
-        <f aca="false">F23+F40</f>
-        <v>-0.0217872</v>
-      </c>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="5"/>
+      <c r="P24" s="5"/>
       <c r="R24" s="8" t="n">
         <f aca="false">M24/SUM(M$3:M$24)</f>
-        <v>-0.000288158284793518</v>
+        <v>0</v>
       </c>
       <c r="S24" s="8" t="n">
         <f aca="false">N24/SUM(N$3:N$24)</f>
-        <v>-0.000256392626076901</v>
+        <v>0</v>
       </c>
       <c r="T24" s="8" t="n">
         <f aca="false">O24/SUM(O$3:O$24)</f>
-        <v>-0.000262645579623251</v>
+        <v>0</v>
       </c>
       <c r="U24" s="8" t="n">
         <f aca="false">P24/SUM(P$3:P$24)</f>
-        <v>-0.000276206998798737</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2430,7 +2431,7 @@
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="7"/>
       <c r="B26" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>2</v>
@@ -2451,7 +2452,7 @@
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="7"/>
       <c r="B27" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C27" s="7" t="n">
         <v>0</v>
@@ -2472,7 +2473,7 @@
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="7"/>
       <c r="B28" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C28" s="7" t="n">
         <v>0</v>
@@ -2493,7 +2494,7 @@
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="7"/>
       <c r="B29" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C29" s="7" t="n">
         <v>4.87728</v>
@@ -2514,7 +2515,7 @@
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="7"/>
       <c r="B30" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C30" s="7" t="n">
         <v>0</v>
@@ -2577,7 +2578,7 @@
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="7"/>
       <c r="B33" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C33" s="7" t="n">
         <v>5</v>
@@ -2619,7 +2620,7 @@
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="7"/>
       <c r="B35" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C35" s="7" t="n">
         <v>0</v>
@@ -2640,7 +2641,7 @@
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="7"/>
       <c r="B36" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C36" s="7" t="n">
         <v>4.83408</v>
@@ -2661,7 +2662,7 @@
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="7"/>
       <c r="B37" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C37" s="7" t="n">
         <v>0</v>
@@ -2681,10 +2682,10 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B38" s="7" t="s">
         <v>45</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>46</v>
       </c>
       <c r="C38" s="7" t="n">
         <v>-0.0005832</v>
@@ -2704,10 +2705,10 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C39" s="7" t="n">
         <v>0.0011088</v>
@@ -2727,24 +2728,12 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="7"/>
-      <c r="B40" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C40" s="7" t="n">
-        <v>-0.0087156</v>
-      </c>
-      <c r="D40" s="7" t="n">
-        <v>-0.0087156</v>
-      </c>
-      <c r="E40" s="7" t="n">
-        <v>-0.0087156</v>
-      </c>
-      <c r="F40" s="7" t="n">
-        <v>-0.0087156</v>
-      </c>
-      <c r="G40" s="7" t="n">
-        <v>-0.0087156</v>
-      </c>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
       <c r="J40" s="5" t="str">
         <f aca="false">B45</f>
         <v>central DH</v>
@@ -2754,7 +2743,7 @@
         <v>decentral DH</v>
       </c>
       <c r="L40" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M40" s="6" t="str">
         <f aca="false">C45</f>
@@ -2772,23 +2761,23 @@
         <f aca="false">F45</f>
         <v>Hydrogen</v>
       </c>
-      <c r="W40" s="0" t="str">
+      <c r="W40" s="5" t="str">
         <f aca="false">L40</f>
         <v>2035 combined district heat</v>
       </c>
-      <c r="X40" s="0" t="str">
+      <c r="X40" s="5" t="str">
         <f aca="false">M40</f>
         <v>Wind</v>
       </c>
-      <c r="Y40" s="0" t="str">
+      <c r="Y40" s="5" t="str">
         <f aca="false">N40</f>
         <v>Biomass</v>
       </c>
-      <c r="Z40" s="0" t="str">
+      <c r="Z40" s="5" t="str">
         <f aca="false">O40</f>
         <v>Bio+</v>
       </c>
-      <c r="AA40" s="0" t="str">
+      <c r="AA40" s="5" t="str">
         <f aca="false">P40</f>
         <v>Hydrogen</v>
       </c>
@@ -2838,13 +2827,13 @@
       </c>
       <c r="T41" s="8" t="n">
         <f aca="false">O41/SUM(O$41:O$62)</f>
-        <v>0.103825740154353</v>
+        <v>0.103808507786306</v>
       </c>
       <c r="U41" s="8" t="n">
         <f aca="false">P41/SUM(P$41:P$62)</f>
         <v>0</v>
       </c>
-      <c r="W41" s="0" t="str">
+      <c r="W41" s="5" t="str">
         <f aca="false">L41</f>
         <v>Woodchips CHP</v>
       </c>
@@ -2902,37 +2891,37 @@
       </c>
       <c r="R42" s="8" t="n">
         <f aca="false">M42/SUM(M$41:M$62)</f>
-        <v>0.0971823578061266</v>
+        <v>0.097163949040585</v>
       </c>
       <c r="S42" s="8" t="n">
         <f aca="false">N42/SUM(N$41:N$62)</f>
-        <v>0.0675863437830336</v>
+        <v>0.0675744912515545</v>
       </c>
       <c r="T42" s="8" t="n">
         <f aca="false">O42/SUM(O$41:O$62)</f>
-        <v>0.0568378605179275</v>
+        <v>0.0568284269137946</v>
       </c>
       <c r="U42" s="8" t="n">
         <f aca="false">P42/SUM(P$41:P$62)</f>
-        <v>0.0469553617001855</v>
-      </c>
-      <c r="W42" s="0" t="str">
+        <v>0.04694881779494</v>
+      </c>
+      <c r="W42" s="5" t="str">
         <f aca="false">L42</f>
         <v>Gas CHP</v>
       </c>
-      <c r="X42" s="0" t="n">
+      <c r="X42" s="5" t="n">
         <f aca="false">M42+M43+M44</f>
         <v>10.24488</v>
       </c>
-      <c r="Y42" s="0" t="n">
+      <c r="Y42" s="5" t="n">
         <f aca="false">N42+N43+N44</f>
         <v>9.69608</v>
       </c>
-      <c r="Z42" s="0" t="n">
+      <c r="Z42" s="5" t="n">
         <f aca="false">O42+O43+O44</f>
         <v>10.83856</v>
       </c>
-      <c r="AA42" s="0" t="n">
+      <c r="AA42" s="5" t="n">
         <f aca="false">P42+P43+P44</f>
         <v>12.7284</v>
       </c>
@@ -2973,17 +2962,17 @@
       </c>
       <c r="S43" s="8" t="n">
         <f aca="false">N43/SUM(N$41:N$62)</f>
-        <v>0.00878191803918795</v>
+        <v>0.00878037796534788</v>
       </c>
       <c r="T43" s="8" t="n">
         <f aca="false">O43/SUM(O$41:O$62)</f>
-        <v>0.0166227569891695</v>
+        <v>0.0166199980445575</v>
       </c>
       <c r="U43" s="8" t="n">
         <f aca="false">P43/SUM(P$41:P$62)</f>
-        <v>0.0209360449884901</v>
-      </c>
-      <c r="W43" s="0" t="str">
+        <v>0.0209331272493936</v>
+      </c>
+      <c r="W43" s="5" t="str">
         <f aca="false">L45</f>
         <v>Waste CHP</v>
       </c>
@@ -3042,17 +3031,17 @@
       </c>
       <c r="S44" s="8" t="n">
         <f aca="false">N44/SUM(N$41:N$62)</f>
-        <v>0.00878191803918795</v>
+        <v>0.00878037796534788</v>
       </c>
       <c r="T44" s="8" t="n">
         <f aca="false">O44/SUM(O$41:O$62)</f>
-        <v>0.0166227569891695</v>
+        <v>0.0166199980445575</v>
       </c>
       <c r="U44" s="8" t="n">
         <f aca="false">P44/SUM(P$41:P$62)</f>
-        <v>0.0209360449884901</v>
-      </c>
-      <c r="W44" s="0" t="str">
+        <v>0.0209331272493936</v>
+      </c>
+      <c r="W44" s="5" t="str">
         <f aca="false">L46</f>
         <v>Biomass</v>
       </c>
@@ -3122,37 +3111,37 @@
       </c>
       <c r="R45" s="8" t="n">
         <f aca="false">M45/SUM(M$41:M$62)</f>
-        <v>0.259724615077942</v>
+        <v>0.259675416749642</v>
       </c>
       <c r="S45" s="8" t="n">
         <f aca="false">N45/SUM(N$41:N$62)</f>
-        <v>0.240338404256361</v>
+        <v>0.240296256414909</v>
       </c>
       <c r="T45" s="8" t="n">
         <f aca="false">O45/SUM(O$41:O$62)</f>
-        <v>0.227408890319864</v>
+        <v>0.22737114636842</v>
       </c>
       <c r="U45" s="8" t="n">
         <f aca="false">P45/SUM(P$41:P$62)</f>
-        <v>0.191163342045985</v>
-      </c>
-      <c r="W45" s="0" t="str">
+        <v>0.191136700683817</v>
+      </c>
+      <c r="W45" s="5" t="str">
         <f aca="false">L48</f>
         <v>heat pumps</v>
       </c>
-      <c r="X45" s="0" t="n">
+      <c r="X45" s="7" t="n">
         <f aca="false">M48</f>
         <v>11.18664</v>
       </c>
-      <c r="Y45" s="0" t="n">
+      <c r="Y45" s="7" t="n">
         <f aca="false">N48</f>
         <v>7.5573</v>
       </c>
-      <c r="Z45" s="0" t="n">
+      <c r="Z45" s="7" t="n">
         <f aca="false">O48</f>
         <v>5.1858</v>
       </c>
-      <c r="AA45" s="0" t="n">
+      <c r="AA45" s="7" t="n">
         <f aca="false">P48</f>
         <v>11.56698</v>
       </c>
@@ -3206,37 +3195,37 @@
       </c>
       <c r="R46" s="8" t="n">
         <f aca="false">M46/SUM(M$41:M$62)</f>
-        <v>0.203720592127042</v>
+        <v>0.203682002359299</v>
       </c>
       <c r="S46" s="8" t="n">
         <f aca="false">N46/SUM(N$41:N$62)</f>
-        <v>0.224916843315533</v>
+        <v>0.224877399933685</v>
       </c>
       <c r="T46" s="8" t="n">
         <f aca="false">O46/SUM(O$41:O$62)</f>
-        <v>0.220070056143894</v>
+        <v>0.220033530247735</v>
       </c>
       <c r="U46" s="8" t="n">
         <f aca="false">P46/SUM(P$41:P$62)</f>
-        <v>0.154497309508859</v>
-      </c>
-      <c r="W46" s="0" t="str">
+        <v>0.154475778085875</v>
+      </c>
+      <c r="W46" s="5" t="str">
         <f aca="false">L49</f>
         <v>Geothermal</v>
       </c>
-      <c r="X46" s="0" t="n">
+      <c r="X46" s="7" t="n">
         <f aca="false">M49</f>
         <v>4.75236</v>
       </c>
-      <c r="Y46" s="0" t="n">
+      <c r="Y46" s="7" t="n">
         <f aca="false">N49</f>
         <v>4.176</v>
       </c>
-      <c r="Z46" s="0" t="n">
+      <c r="Z46" s="7" t="n">
         <f aca="false">O49</f>
         <v>4.00752</v>
       </c>
-      <c r="AA46" s="0" t="n">
+      <c r="AA46" s="7" t="n">
         <f aca="false">P49</f>
         <v>4.8204</v>
       </c>
@@ -3244,7 +3233,7 @@
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="7"/>
       <c r="B47" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C47" s="7" t="n">
         <v>21.4760484</v>
@@ -3304,23 +3293,23 @@
         <f aca="false">P47/SUM(P$41:P$62)</f>
         <v>0</v>
       </c>
-      <c r="W47" s="0" t="str">
+      <c r="W47" s="5" t="str">
         <f aca="false">L50</f>
         <v>Solar heat</v>
       </c>
-      <c r="X47" s="0" t="n">
+      <c r="X47" s="7" t="n">
         <f aca="false">M50</f>
         <v>3.5</v>
       </c>
-      <c r="Y47" s="0" t="n">
+      <c r="Y47" s="7" t="n">
         <f aca="false">N50</f>
         <v>3.5</v>
       </c>
-      <c r="Z47" s="0" t="n">
+      <c r="Z47" s="7" t="n">
         <f aca="false">O50</f>
         <v>3.5</v>
       </c>
-      <c r="AA47" s="0" t="n">
+      <c r="AA47" s="7" t="n">
         <f aca="false">P50</f>
         <v>3.5</v>
       </c>
@@ -3328,7 +3317,7 @@
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="7"/>
       <c r="B48" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C48" s="7" t="n">
         <v>0</v>
@@ -3375,37 +3364,37 @@
       </c>
       <c r="R48" s="8" t="n">
         <f aca="false">M48/SUM(M$41:M$62)</f>
-        <v>0.106115840412804</v>
+        <v>0.106095739422557</v>
       </c>
       <c r="S48" s="8" t="n">
         <f aca="false">N48/SUM(N$41:N$62)</f>
-        <v>0.0663675891975551</v>
+        <v>0.0663559503975235</v>
       </c>
       <c r="T48" s="8" t="n">
         <f aca="false">O48/SUM(O$41:O$62)</f>
-        <v>0.0431011465972176</v>
+        <v>0.0430939929297332</v>
       </c>
       <c r="U48" s="8" t="n">
         <f aca="false">P48/SUM(P$41:P$62)</f>
-        <v>0.0807222712203216</v>
-      </c>
-      <c r="W48" s="0" t="str">
+        <v>0.080711021410397</v>
+      </c>
+      <c r="W48" s="5" t="str">
         <f aca="false">L51</f>
         <v>Residual industrial heat</v>
       </c>
-      <c r="X48" s="0" t="n">
+      <c r="X48" s="7" t="n">
         <f aca="false">M51</f>
         <v>4.7</v>
       </c>
-      <c r="Y48" s="0" t="n">
+      <c r="Y48" s="7" t="n">
         <f aca="false">N51</f>
         <v>4.7</v>
       </c>
-      <c r="Z48" s="0" t="n">
+      <c r="Z48" s="7" t="n">
         <f aca="false">O51</f>
         <v>4.7</v>
       </c>
-      <c r="AA48" s="0" t="n">
+      <c r="AA48" s="7" t="n">
         <f aca="false">P51</f>
         <v>4.7</v>
       </c>
@@ -3413,7 +3402,7 @@
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="7"/>
       <c r="B49" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C49" s="7" t="n">
         <v>0</v>
@@ -3460,37 +3449,37 @@
       </c>
       <c r="R49" s="8" t="n">
         <f aca="false">M49/SUM(M$41:M$62)</f>
-        <v>0.0450806207533445</v>
+        <v>0.0450720813579578</v>
       </c>
       <c r="S49" s="8" t="n">
         <f aca="false">N49/SUM(N$41:N$62)</f>
-        <v>0.0366732897316489</v>
+        <v>0.0366668583832927</v>
       </c>
       <c r="T49" s="8" t="n">
         <f aca="false">O49/SUM(O$41:O$62)</f>
-        <v>0.0333080155446183</v>
+        <v>0.0333024872817625</v>
       </c>
       <c r="U49" s="8" t="n">
         <f aca="false">P49/SUM(P$41:P$62)</f>
-        <v>0.0336400370875058</v>
-      </c>
-      <c r="W49" s="0" t="str">
+        <v>0.0336353488643256</v>
+      </c>
+      <c r="W49" s="5" t="str">
         <f aca="false">L52</f>
         <v>Wood boiler</v>
       </c>
-      <c r="X49" s="0" t="n">
+      <c r="X49" s="7" t="n">
         <f aca="false">M52</f>
         <v>0</v>
       </c>
-      <c r="Y49" s="0" t="n">
+      <c r="Y49" s="7" t="n">
         <f aca="false">N52</f>
         <v>26.28216</v>
       </c>
-      <c r="Z49" s="0" t="n">
+      <c r="Z49" s="7" t="n">
         <f aca="false">O52</f>
         <v>15.77376</v>
       </c>
-      <c r="AA49" s="0" t="n">
+      <c r="AA49" s="7" t="n">
         <f aca="false">P52</f>
         <v>0</v>
       </c>
@@ -3545,37 +3534,37 @@
       </c>
       <c r="R50" s="8" t="n">
         <f aca="false">M50/SUM(M$41:M$62)</f>
-        <v>0.0332008039451358</v>
+        <v>0.0331945148837319</v>
       </c>
       <c r="S50" s="8" t="n">
         <f aca="false">N50/SUM(N$41:N$62)</f>
-        <v>0.0307367131371578</v>
+        <v>0.0307313228787176</v>
       </c>
       <c r="T50" s="8" t="n">
         <f aca="false">O50/SUM(O$41:O$62)</f>
-        <v>0.0290898247310466</v>
+        <v>0.0290849965779756</v>
       </c>
       <c r="U50" s="8" t="n">
         <f aca="false">P50/SUM(P$41:P$62)</f>
-        <v>0.0244253858199051</v>
-      </c>
-      <c r="W50" s="0" t="str">
+        <v>0.0244219817909592</v>
+      </c>
+      <c r="W50" s="5" t="str">
         <f aca="false">L53</f>
         <v>Straw boiler</v>
       </c>
-      <c r="X50" s="0" t="n">
+      <c r="X50" s="7" t="n">
         <f aca="false">M53</f>
         <v>22.19868</v>
       </c>
-      <c r="Y50" s="0" t="n">
+      <c r="Y50" s="7" t="n">
         <f aca="false">N53</f>
         <v>0</v>
       </c>
-      <c r="Z50" s="0" t="n">
+      <c r="Z50" s="7" t="n">
         <f aca="false">O53</f>
         <v>0</v>
       </c>
-      <c r="AA50" s="0" t="n">
+      <c r="AA50" s="7" t="n">
         <f aca="false">P53</f>
         <v>41.46624</v>
       </c>
@@ -3630,36 +3619,36 @@
       </c>
       <c r="R51" s="8" t="n">
         <f aca="false">M51/SUM(M$41:M$62)</f>
-        <v>0.0445839367263252</v>
+        <v>0.0445754914152972</v>
       </c>
       <c r="S51" s="8" t="n">
         <f aca="false">N51/SUM(N$41:N$62)</f>
-        <v>0.0412750147841834</v>
+        <v>0.041267776437135</v>
       </c>
       <c r="T51" s="8" t="n">
         <f aca="false">O51/SUM(O$41:O$62)</f>
-        <v>0.0390634789245483</v>
+        <v>0.0390569954047101</v>
       </c>
       <c r="U51" s="8" t="n">
         <f aca="false">P51/SUM(P$41:P$62)</f>
-        <v>0.0327998038153011</v>
-      </c>
-      <c r="W51" s="0" t="s">
+        <v>0.0327952326907167</v>
+      </c>
+      <c r="W51" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="X51" s="0" t="n">
+      <c r="X51" s="5" t="n">
         <f aca="false">M55+M56+M57+M58+M59</f>
         <v>0</v>
       </c>
-      <c r="Y51" s="0" t="n">
+      <c r="Y51" s="5" t="n">
         <f aca="false">N55+N56+N57+N58+N59</f>
         <v>5</v>
       </c>
-      <c r="Z51" s="0" t="n">
+      <c r="Z51" s="5" t="n">
         <f aca="false">O55+O56+O57+O58+O59</f>
         <v>10</v>
       </c>
-      <c r="AA51" s="0" t="n">
+      <c r="AA51" s="5" t="n">
         <f aca="false">P55+P56+P57+P58+P59</f>
         <v>15</v>
       </c>
@@ -3667,7 +3656,7 @@
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="7"/>
       <c r="B52" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C52" s="7" t="n">
         <v>1</v>
@@ -3718,36 +3707,20 @@
       </c>
       <c r="S52" s="8" t="n">
         <f aca="false">N52/SUM(N$41:N$62)</f>
-        <v>0.230807775012824</v>
+        <v>0.230767298545747</v>
       </c>
       <c r="T52" s="8" t="n">
         <f aca="false">O52/SUM(O$41:O$62)</f>
-        <v>0.131101689642741</v>
+        <v>0.13107993017766</v>
       </c>
       <c r="U52" s="8" t="n">
         <f aca="false">P52/SUM(P$41:P$62)</f>
         <v>0</v>
       </c>
-      <c r="W52" s="0" t="str">
-        <f aca="false">L62</f>
-        <v>District heat use</v>
-      </c>
-      <c r="X52" s="0" t="n">
-        <f aca="false">M62</f>
-        <v>-0.0199728</v>
-      </c>
-      <c r="Y52" s="0" t="n">
-        <f aca="false">N62</f>
-        <v>-0.0199728</v>
-      </c>
-      <c r="Z52" s="0" t="n">
-        <f aca="false">O62</f>
-        <v>-0.0199728</v>
-      </c>
-      <c r="AA52" s="0" t="n">
-        <f aca="false">P62</f>
-        <v>-0.0199728</v>
-      </c>
+      <c r="X52" s="7"/>
+      <c r="Y52" s="7"/>
+      <c r="Z52" s="7"/>
+      <c r="AA52" s="7"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="7"/>
@@ -3799,7 +3772,7 @@
       </c>
       <c r="R53" s="8" t="n">
         <f aca="false">M53/SUM(M$41:M$62)</f>
-        <v>0.210575435005945</v>
+        <v>0.210535546759772</v>
       </c>
       <c r="S53" s="8" t="n">
         <f aca="false">N53/SUM(N$41:N$62)</f>
@@ -3811,7 +3784,7 @@
       </c>
       <c r="U53" s="8" t="n">
         <f aca="false">P53/SUM(P$41:P$62)</f>
-        <v>0.289379688714509</v>
+        <v>0.289339359491298</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3927,21 +3900,21 @@
       </c>
       <c r="S55" s="8" t="n">
         <f aca="false">N55/SUM(N$41:N$62)</f>
-        <v>0.00878191803918795</v>
+        <v>0.00878037796534788</v>
       </c>
       <c r="T55" s="8" t="n">
         <f aca="false">O55/SUM(O$41:O$62)</f>
-        <v>0.0166227569891695</v>
+        <v>0.0166199980445575</v>
       </c>
       <c r="U55" s="8" t="n">
         <f aca="false">P55/SUM(P$41:P$62)</f>
-        <v>0.0209360449884901</v>
+        <v>0.0209331272493936</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="7"/>
       <c r="B56" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C56" s="7" t="n">
         <v>0</v>
@@ -3986,21 +3959,21 @@
       </c>
       <c r="S56" s="8" t="n">
         <f aca="false">N56/SUM(N$41:N$62)</f>
-        <v>0.00878191803918795</v>
+        <v>0.00878037796534788</v>
       </c>
       <c r="T56" s="8" t="n">
         <f aca="false">O56/SUM(O$41:O$62)</f>
-        <v>0.0166227569891695</v>
+        <v>0.0166199980445575</v>
       </c>
       <c r="U56" s="8" t="n">
         <f aca="false">P56/SUM(P$41:P$62)</f>
-        <v>0.0209360449884901</v>
+        <v>0.0209331272493936</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="7"/>
       <c r="B57" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C57" s="7" t="n">
         <v>0.0002772</v>
@@ -4045,21 +4018,21 @@
       </c>
       <c r="S57" s="8" t="n">
         <f aca="false">N57/SUM(N$41:N$62)</f>
-        <v>0.00878191803918795</v>
+        <v>0.00878037796534788</v>
       </c>
       <c r="T57" s="8" t="n">
         <f aca="false">O57/SUM(O$41:O$62)</f>
-        <v>0.0166227569891695</v>
+        <v>0.0166199980445575</v>
       </c>
       <c r="U57" s="8" t="n">
         <f aca="false">P57/SUM(P$41:P$62)</f>
-        <v>0.0209360449884901</v>
+        <v>0.0209331272493936</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="7"/>
       <c r="B58" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C58" s="7" t="n">
         <v>0</v>
@@ -4104,37 +4077,25 @@
       </c>
       <c r="S58" s="8" t="n">
         <f aca="false">N58/SUM(N$41:N$62)</f>
-        <v>0.00878191803918795</v>
+        <v>0.00878037796534788</v>
       </c>
       <c r="T58" s="8" t="n">
         <f aca="false">O58/SUM(O$41:O$62)</f>
-        <v>0.0166227569891695</v>
+        <v>0.0166199980445575</v>
       </c>
       <c r="U58" s="8" t="n">
         <f aca="false">P58/SUM(P$41:P$62)</f>
-        <v>0.0209360449884901</v>
+        <v>0.0209331272493936</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="7"/>
-      <c r="B59" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C59" s="7" t="n">
-        <v>-0.0099864</v>
-      </c>
-      <c r="D59" s="7" t="n">
-        <v>-0.0099864</v>
-      </c>
-      <c r="E59" s="7" t="n">
-        <v>-0.0099864</v>
-      </c>
-      <c r="F59" s="7" t="n">
-        <v>-0.0099864</v>
-      </c>
-      <c r="G59" s="7" t="n">
-        <v>-0.0099864</v>
-      </c>
+      <c r="B59" s="7"/>
+      <c r="C59" s="7"/>
+      <c r="D59" s="7"/>
+      <c r="E59" s="7"/>
+      <c r="F59" s="7"/>
+      <c r="G59" s="7"/>
       <c r="J59" s="5" t="s">
         <v>17</v>
       </c>
@@ -4163,15 +4124,15 @@
       </c>
       <c r="S59" s="8" t="n">
         <f aca="false">N59/SUM(N$41:N$62)</f>
-        <v>0.00878191803918795</v>
+        <v>0.00878037796534788</v>
       </c>
       <c r="T59" s="8" t="n">
         <f aca="false">O59/SUM(O$41:O$62)</f>
-        <v>0.0166227569891695</v>
+        <v>0.0166199980445575</v>
       </c>
       <c r="U59" s="8" t="n">
         <f aca="false">P59/SUM(P$41:P$62)</f>
-        <v>0.0209360449884901</v>
+        <v>0.0209331272493936</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4212,7 +4173,7 @@
       </c>
       <c r="R60" s="8" t="n">
         <f aca="false">M60/SUM(M$41:M$62)</f>
-        <v>5.25900734490951E-006</v>
+        <v>5.25801115758314E-006</v>
       </c>
       <c r="S60" s="8" t="n">
         <f aca="false">N60/SUM(N$41:N$62)</f>
@@ -4224,7 +4185,7 @@
       </c>
       <c r="U60" s="8" t="n">
         <f aca="false">P60/SUM(P$41:P$62)</f>
-        <v>3.86898111387296E-006</v>
+        <v>3.86844191568794E-006</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4285,7 +4246,7 @@
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="7"/>
       <c r="B62" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C62" s="7" t="s">
         <v>2</v>
@@ -4302,55 +4263,34 @@
       <c r="G62" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="J62" s="5" t="str">
-        <f aca="false">B59</f>
-        <v>District heat use</v>
-      </c>
-      <c r="K62" s="1" t="str">
-        <f aca="false">B74</f>
-        <v>District heat use</v>
-      </c>
-      <c r="L62" s="6" t="str">
-        <f aca="false">L24</f>
-        <v>District heat use</v>
-      </c>
-      <c r="M62" s="7" t="n">
-        <f aca="false">C59+C74</f>
-        <v>-0.0199728</v>
-      </c>
-      <c r="N62" s="7" t="n">
-        <f aca="false">D59+D74</f>
-        <v>-0.0199728</v>
-      </c>
-      <c r="O62" s="7" t="n">
-        <f aca="false">E59+E74</f>
-        <v>-0.0199728</v>
-      </c>
-      <c r="P62" s="7" t="n">
-        <f aca="false">F59+F74</f>
-        <v>-0.0199728</v>
-      </c>
+      <c r="J62" s="5"/>
+      <c r="K62" s="1"/>
+      <c r="L62" s="6"/>
+      <c r="M62" s="7"/>
+      <c r="N62" s="7"/>
+      <c r="O62" s="7"/>
+      <c r="P62" s="7"/>
       <c r="R62" s="8" t="n">
         <f aca="false">M62/SUM(M$41:M$62)</f>
-        <v>-0.000189460862010117</v>
+        <v>0</v>
       </c>
       <c r="S62" s="8" t="n">
         <f aca="false">N62/SUM(N$41:N$62)</f>
-        <v>-0.000175399492613093</v>
+        <v>0</v>
       </c>
       <c r="T62" s="8" t="n">
         <f aca="false">O62/SUM(O$41:O$62)</f>
-        <v>-0.000166001500396642</v>
+        <v>0</v>
       </c>
       <c r="U62" s="8" t="n">
         <f aca="false">P62/SUM(P$41:P$62)</f>
-        <v>-0.000139383813115371</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="7"/>
       <c r="B63" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C63" s="7" t="n">
         <v>0</v>
@@ -4388,7 +4328,7 @@
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="7"/>
       <c r="B64" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C64" s="7" t="n">
         <v>10.24488</v>
@@ -4451,7 +4391,7 @@
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="7"/>
       <c r="B67" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C67" s="7" t="n">
         <v>2.5</v>
@@ -4535,7 +4475,7 @@
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="7"/>
       <c r="B71" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C71" s="7" t="n">
         <v>0</v>
@@ -4556,7 +4496,7 @@
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="7"/>
       <c r="B72" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C72" s="7" t="n">
         <v>0.0002772</v>
@@ -4577,7 +4517,7 @@
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="7"/>
       <c r="B73" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C73" s="7" t="n">
         <v>0</v>
@@ -4597,24 +4537,12 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="7"/>
-      <c r="B74" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C74" s="7" t="n">
-        <v>-0.0099864</v>
-      </c>
-      <c r="D74" s="7" t="n">
-        <v>-0.0099864</v>
-      </c>
-      <c r="E74" s="7" t="n">
-        <v>-0.0099864</v>
-      </c>
-      <c r="F74" s="7" t="n">
-        <v>-0.0099864</v>
-      </c>
-      <c r="G74" s="7" t="n">
-        <v>-0.0099864</v>
-      </c>
+      <c r="B74" s="7"/>
+      <c r="C74" s="7"/>
+      <c r="D74" s="7"/>
+      <c r="E74" s="7"/>
+      <c r="F74" s="7"/>
+      <c r="G74" s="7"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="R41:U63 R3:U25">
@@ -4635,4 +4563,104 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.58"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="6" t="n">
+        <v>2035</v>
+      </c>
+      <c r="C1" s="6" t="n">
+        <v>2050</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <f aca="false">4161+2774</f>
+        <v>6935</v>
+      </c>
+      <c r="C2" s="12" t="n">
+        <f aca="false">3631+2421</f>
+        <v>6052</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>74.2</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>68.8</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <f aca="false">5016</f>
+        <v>5016</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <f aca="false">6162</f>
+        <v>6162</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <f aca="false">B3/B2*B4</f>
+        <v>53.6679452054795</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <f aca="false">C3/C2*C4</f>
+        <v>70.0504957038995</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>